<commit_message>
Added URI functionality to the converter.
Users can now submit a URI as a parameter in the temp.py file.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -904,12 +904,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>http://examples.org/SA_u45_aMF_u916_/1</t>
+          <t>http://examples.org/Inulinase_u45_aMF_u916_/1</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SA-aMFΔ</t>
+          <t>Inulinase-aMFΔ</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -922,7 +922,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Serum albumin followed by aMFΔ</t>
+          <t>Inulinase followed by aMFΔ</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -935,7 +935,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>atgaagtgggtaactttcatctcattgttattcttgttctcctctgcttactctatgagatttcctagtattttcactgctgtgctatttgcctctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatctctagagaagcgt</t>
+          <t>atgaaactggcttactccctgttgctacctctggctggagtttccgctatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatctctagagaagcgt</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -948,32 +948,32 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>http://examples.org/aMF_u916__no_Kex/1</t>
+          <t>http://examples.org/yEGFP/1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>aMFΔ_no_Kex</t>
+          <t>yEGFP</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>signal_peptide_region_of_CDS</t>
+          <t>CDS</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>No Kex recognition site</t>
+          <t>No stop codon</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>α-mating factor no Kex recognition site</t>
+          <t>Green fluorescent protein</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Saccharomyces cerevisiae</t>
+          <t>Aequorea victoria</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -983,7 +983,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>atgagattcccatcaatttttactgctgttctgttcgccgcttctagtgcacttgccatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcacagccaaggaagaaggtgtatctctagagaagcgt</t>
+          <t>atggtgagcaagggcgaggagctgttcaccggggtggtgcccatcctggtcgagctggacggcgacgtaaacggccacaagttcagcgtgtccggcgagggcgagggcgatgccacctacggcaagctgaccctgaagttcatctgcaccaccggcaagctgcccgtgccctggcccaccctcgtgaccaccctgacctacggcgtgcagtgcttcagccgctaccccgaccacatgaagcagcacgacttcttcaagtccgccatgcccgaaggctacgtccaggagcgcaccatcttcttcaaggacgacggcaactacaagacccgcgccgaggtgaagttcgagggcgacaccctggtgaaccgcatcgagctgaagggcatcgacttcaaggaggacggcaacatcctggggcacaagctggagtacaactacaacagccacaacgtctatatcatggccgacaagcagaagaacggcatcaaggtgaacttcaagatccgccacaacatcgaggacggcagcgtgcagctcgccgaccactaccagcagaacacccccatcggcgacggccccgtgctgctgcccgacaaccactacctgagcacccagagcgccctgagcaaagaccccaacgagaagcgcgatcacatggtcctgctggagttcgtgaccgccgccgggatcactctcggcatggacgagctgtacaag</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -993,39 +993,39 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://synbiohub.org/public/Excel2SBOL/Truncated/1</t>
+          <t>https://synbiohub.org/public/Excel2SBOL/codon_optimisation/1</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>http://examples.org/RFP/1</t>
+          <t>http://examples.org/aMF_u916_/1</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>RFP</t>
+          <t>aMFΔ</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>CDS</t>
+          <t>signal_peptide_region_of_CDS</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>No stop codon</t>
+          <t>Pre-sequence shortened</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Red fluorescent protein, BsaI removed</t>
+          <t>α-mating factor, pre-sequence shortened</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Discosoma sp.</t>
+          <t>Saccharomyces cerevisiae</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1035,7 +1035,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>atcgcaacttccggtatggtgtcaaagggagaggaaaataatatggctattattaaggagtttatgcgttttaaggtacatatggaaggttctgtcaacggtcacgaattcgaaattgaaggtgagggggaggggaggccatacgagggaactcagactgctaagttaaaggtcactaaaggtggtcctttacctttcgcctgggatatcctgtctccacagtttatgtacggttcaaaggcttatgtgaaacatcctgccgatatcccagattatcttaaactttctttccctgagggttttaagtgggagagggtaatgaactttgaagacggtggtgtggtcactgttactcaggactcaagtctgcaggacggtgagttcatctacaaggtgaagctgagaggtaccaattttccatcagatggtcccgtgatgcaaaaaaagacaatgggttgggaagcttctagtgaacgtatgtatcccgaagatggagctttgaaaggtgaaattaagcaaagactaaaacttaaggatggtggacattacgatgctgaagttaagacgacctacaaggccaaaaagccagtccagttgcctggagcatacaatgttaacatcaaattggatataacttcccataatgaagactataccatcgtcgagcaatacgaacgagccgaagggagacacagtactggtggtatggatgaactttataaaggatccggaaccgca</t>
+          <t>atgagatttcctagtattttcactgctgtgctatttgccgctagttcc</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1045,36 +1045,40 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://synbiohub.org/public/Excel2SBOL/mutations/1</t>
+          <t>https://synbiohub.org/public/Excel2SBOL/Truncated/1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>http://examples.org/aAmylase_u45_aMF_u916_/1</t>
+          <t>http://examples.org/RFP_Sec/1</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>aAmylase-aMFΔ</t>
+          <t>RFP_Sec</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>signal_peptide_region_of_CDS</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v/>
+          <t>CDS</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>No start or stop codon, for use with N-terminal secretion tag</t>
+        </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>α-Amylase followed by aMFΔ</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
-        <v/>
+          <t>Red fluorescent protein, BsaI removed</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Discosoma sp.</t>
+        </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1083,7 +1087,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>atggtggcatggtggtccttattcttatatggtcttcaagttgctgctcctgcccttgctatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatctctagagaagcgt</t>
+          <t>gcaacttccggtatggtgtcaaagggagaggaaaataatatggctattattaaggagtttatgcgttttaaggtacatatggaaggttctgtcaacggtcacgaattcgaaattgaaggtgagggggaggggaggccatacgagggaactcagactgctaagttaaaggtcactaaaggtggtcctttacctttcgcctgggatatcctgtctccacagtttatgtacggttcaaaggcttatgtgaaacatcctgccgatatcccagattatcttaaactttctttccctgagggttttaagtgggagagggtaatgaactttgaagacggtggtgtggtcactgttactcaggactcaagtctgcaggacggtgagttcatctacaaggtgaagctgagaggtaccaattttccatcagatggtcccgtgatgcaaaaaaagacaatgggttgggaagcttctagtgaacgtatgtatcccgaagatggagctttgaaaggtgaaattaagcaaagactaaaacttaaggatggtggacattacgatgctgaagttaagacgacctacaaggccaaaaagccagtccagttgcctggagcatacaatgttaacatcaaattggatataacttcccataatgaagactataccatcgtcgagcaatacgaacgagccgaagggagacacagtactggtggtatggatgaactttataaaggatccggaaccgca</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1093,19 +1097,19 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://synbiohub.org/public/Excel2SBOL/Composite/1</t>
+          <t>https://synbiohub.org/public/Excel2SBOL/mutations/1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>http://examples.org/Glucoamylase_u45_aMF_u916_/1</t>
+          <t>http://examples.org/SA_u45_aMF_u916_/1</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Glucoamylase-aMFΔ</t>
+          <t>SA-aMFΔ</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1118,7 +1122,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Glucoamylase followed by aMFΔ</t>
+          <t>Serum albumin followed by aMFΔ</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1131,7 +1135,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>atgtctttcagatccctattggcattgtcagggttggtctgttctggattggctatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatctctagagaagcgt</t>
+          <t>atgaagtgggtaactttcatctcattgttattcttgttctcctctgcttactctatgagatttcctagtattttcactgctgtgctatttgcctctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatctctagagaagcgt</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1144,12 +1148,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>http://examples.org/yEGFP/1</t>
+          <t>http://examples.org/RFP/1</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>yEGFP</t>
+          <t>RFP</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1164,12 +1168,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Green fluorescent protein</t>
+          <t>Red fluorescent protein, BsaI removed</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Aequorea victoria</t>
+          <t>Discosoma sp.</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1179,7 +1183,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>atggtgagcaagggcgaggagctgttcaccggggtggtgcccatcctggtcgagctggacggcgacgtaaacggccacaagttcagcgtgtccggcgagggcgagggcgatgccacctacggcaagctgaccctgaagttcatctgcaccaccggcaagctgcccgtgccctggcccaccctcgtgaccaccctgacctacggcgtgcagtgcttcagccgctaccccgaccacatgaagcagcacgacttcttcaagtccgccatgcccgaaggctacgtccaggagcgcaccatcttcttcaaggacgacggcaactacaagacccgcgccgaggtgaagttcgagggcgacaccctggtgaaccgcatcgagctgaagggcatcgacttcaaggaggacggcaacatcctggggcacaagctggagtacaactacaacagccacaacgtctatatcatggccgacaagcagaagaacggcatcaaggtgaacttcaagatccgccacaacatcgaggacggcagcgtgcagctcgccgaccactaccagcagaacacccccatcggcgacggccccgtgctgctgcccgacaaccactacctgagcacccagagcgccctgagcaaagaccccaacgagaagcgcgatcacatggtcctgctggagttcgtgaccgccgccgggatcactctcggcatggacgagctgtacaag</t>
+          <t>atcgcaacttccggtatggtgtcaaagggagaggaaaataatatggctattattaaggagtttatgcgttttaaggtacatatggaaggttctgtcaacggtcacgaattcgaaattgaaggtgagggggaggggaggccatacgagggaactcagactgctaagttaaaggtcactaaaggtggtcctttacctttcgcctgggatatcctgtctccacagtttatgtacggttcaaaggcttatgtgaaacatcctgccgatatcccagattatcttaaactttctttccctgagggttttaagtgggagagggtaatgaactttgaagacggtggtgtggtcactgttactcaggactcaagtctgcaggacggtgagttcatctacaaggtgaagctgagaggtaccaattttccatcagatggtcccgtgatgcaaaaaaagacaatgggttgggaagcttctagtgaacgtatgtatcccgaagatggagctttgaaaggtgaaattaagcaaagactaaaacttaaggatggtggacattacgatgctgaagttaagacgacctacaaggccaaaaagccagtccagttgcctggagcatacaatgttaacatcaaattggatataacttcccataatgaagactataccatcgtcgagcaatacgaacgagccgaagggagacacagtactggtggtatggatgaactttataaaggatccggaaccgca</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1189,24 +1193,24 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://synbiohub.org/public/Excel2SBOL/codon_optimisation/1</t>
+          <t>https://synbiohub.org/public/Excel2SBOL/mutations/1</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>http://examples.org/pAOX1/1</t>
+          <t>http://examples.org/Invertase_u45_aMF_u916_/1</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>pAOX1</t>
+          <t>Invertase-aMFΔ</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>promoter</t>
+          <t>signal_peptide_region_of_CDS</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1214,22 +1218,20 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Alcohol oxidase 1</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
+          <t>Invertase followed by aMFΔ</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v/>
+      </c>
+      <c r="G26" t="inlineStr">
         <is>
           <t>Pichia pastoris</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Pichia pastoris</t>
-        </is>
-      </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>gatctaacatccaaagacgaaaggttgaatgaaacctttttgccatccgacatccacaggtccattctcacacataagtgccaaacgcaacaggaggggatacactagcagcagaccgttgcaaacgcaggacctccactcctcttctcctcaacacccacttttgccatcgaaaaaccagcccagttattgggcttgattggagctcgctcattccaattccttctattaggctactaacaccatgactttattagcctgtctatcctggcccccctggcgaggttcatgtttgtttatttccgaatgcaacaagctccgcattacacccgaacatcactccagatgagggctttctgagtgtggggtcaaatagtttcatgttccccaaatggcccaaaactgacagtttaaacgctgtcttggaacctaatatgacaaaagcgtgatctcatccaagatgaactaagtttggttcgttgaaatgctaacggccagttggtcaaaaagaaacttccaaaagtcggcataccgtttgtcttgtttggtattgattgacgaatgctcaaaaataatctcattaatgcttagcgcagtctctctatcgcttctgaaccccggtgcacctgtgccgaaacgcaaatggggaaacacccgctttttggatgattatgcattgtctccacattgtatgcttccaagattctggtgggaatactgctgatagcctaacgttcatgatcaaaatttaactgttctaacccctacttgacagcaatatataaacagaaggaagctgccctgtcttaaacctttttttttatcatcattattagcttactttcataattgcgactggttccaattgacaagcttttgattttaacgacttttaacgacaacttgagaagatcaaaaaacaactaattattcgaaacg</t>
+          <t>atgttattgcaagcttttttatttctgctggcaggttttgcagcaaagatttctgccatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatctctagagaagcgt</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1237,21 +1239,17 @@
           <t>https://pubmed.ncbi.nlm.nih.gov/28252957</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>https://synbiohub.org/public/Excel2SBOL/direct/1</t>
-        </is>
-      </c>
+      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>http://examples.org/Invertase_u45_aMF_u916_/1</t>
+          <t>http://examples.org/Glucoamylase_u45_aMF_u916_/1</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Invertase-aMFΔ</t>
+          <t>Glucoamylase-aMFΔ</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1264,7 +1262,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Invertase followed by aMFΔ</t>
+          <t>Glucoamylase followed by aMFΔ</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1277,7 +1275,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>atgttattgcaagcttttttatttctgctggcaggttttgcagcaaagatttctgccatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatctctagagaagcgt</t>
+          <t>atgtctttcagatccctattggcattgtcagggttggtctgttctggattggctatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatctctagagaagcgt</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1290,25 +1288,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>http://examples.org/aMF/1</t>
+          <t>http://examples.org/pENO1/1</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>aMF</t>
+          <t>pENO1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>signal_peptide_region_of_CDS</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v/>
+          <t>promoter</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>BsaI and BsmBI site removed</t>
+        </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>α-mating factor</t>
+          <t>Enolase 1</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>atgagatttccttcaatttttactgctgttttattcgcagcatcctccgcattagctgctccagtcaacactacaacagaagatgaaacggcacaaattccggctgaagctgtcatcggttactcagatttagaaggggatttcgatgttgctgttttgccattttccaacagcacaaataacgggttattgtttataaatactactattgccagcattgctgctaaagaagaaggggtatctctcgagaaaagagaggctgaagct</t>
+          <t>agaaagcatactatactattcgacattcctttcaatcctggaattaacagtcacttttaaaaaagacatctaccgtgaaggtgccgtagagtatcgcgttaccatatcgccaaaaactgatatacgccgcggaaaccaggcaaacaattgaaaagaaaaattttgaggaactctctgcatcgaagccgtctagagttaccactagtcagatgccgcgggcacttgagcacctcatgcacagcaataacacaacacaatggttagtagcaacctgaattcggtcattgatgcatgcatgtgccgtgaagcgggacaaccagaaaagtcgtctataaatgccggcacgtgcgatcatcgtggcggggttttaagagtgcatatcacaaattgtcgcattaccgcggaaccgccagatattcattacttgacgcaaaagcgtttgaaataatgacgaaaaagaaggaagaaaaaaaaagaaaaataccgcttctaggcgggttatctactgatccgagcttccactaggatagcacccaaacacctgcatatttggacgacctttacttacaccaccaaaaaccactttcgcctctcccgcccctgataacgtccactaattgagcgattacctgagcggtcctcttttgtttgcagcatgagacttgcatactgcaaatcgtaagtagcaacctctcaaggtcaaaactgtatggaaaccttgtcacctcacttaattctagctagcctaccctgcaagtcaagagctctccgtgattcctagccacctcaaggtatgcctctccccggaaactgtggccttttctggcacacatgatctccacgatttcaacatataaatagcttttgataatggcaatattaatcaaatttattttacttctttcttgtaacatctctcttgtaatcccttattccttctagctatttttcataaaaaaccaagcaactgcttatcaacacacaaacactaaatcaaa</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -1340,17 +1340,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>http://examples.org/tAOX1/1</t>
+          <t>http://examples.org/Killer_u45_aMF_u916_/1</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>tAOX1</t>
+          <t>Killer-aMFΔ</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>terminator</t>
+          <t>signal_peptide_region_of_CDS</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1358,22 +1358,20 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Alcohol oxidase 1</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
+          <t>Killer followed by aMFΔ</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v/>
+      </c>
+      <c r="G29" t="inlineStr">
         <is>
           <t>Pichia pastoris</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Pichia pastoris</t>
-        </is>
-      </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>tcaagaggatgtcagaatgccatttgcctgagagatgcaggcttcatttttgatacttttttatttgtaacctatatagtataggattttttttgtcattttgtttcttctcgtacgagcttgctcctgatcagcctatctcgcagctgatgaatatcttgtggtaggggtttgggaaaatcattcgagtttgatgtttttcttggtatttcccactcctcttcagagtacagaagattaagtgaga</t>
+          <t>atgaccaaaccaacgcaagtcttagttcgttcagtctctattttattcttcatcacactgttgcacttggttgttgcaatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatctctagagaagcgt</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -1381,41 +1379,37 @@
           <t>https://pubmed.ncbi.nlm.nih.gov/28252957</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>https://synbiohub.org/public/Excel2SBOL/direct/1</t>
-        </is>
-      </c>
+      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>http://examples.org/aMF_no_EAEA/1</t>
+          <t>http://examples.org/pGAP/1</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>aMF_no_EAEA</t>
+          <t>pGAP</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>signal_peptide_region_of_CDS</t>
+          <t>promoter</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>No EAEA</t>
+          <t>BsaI site removed</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>α-mating factor no EAEA</t>
+          <t>Glyceraldehyde-3-phosphate dehydrogenase</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Saccharomyces cerevisiae</t>
+          <t>Pichia pastoris</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1425,7 +1419,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>atgagatttccttcaatttttactgctgttttattcgcagcatcctccgcattagctgctccagtcaacactacaacagaagatgaaacggcacaaattccggctgaagctgtcatcggttactcagatttagaaggggatttcgatgttgctgttttgccattttccaacagcacaaataacgggttattgtttataaatactactattgccagcattgctgctaaagaagaaggggtatctctcgagaaaagag</t>
+          <t>tttttgtagaaatgtcttggtgtcctcgtccaatcaggtagccatctctgaaatatctggctccgttgcaactccgaacgacctgctggcaacgtaaaattctccggggtaaaacttaaatgtggagtaatggaaccagaaacgtgtcttcccttctctctccttccaccgcccgttaccgtccctaggaaattttactctgctggagagcttcttctacggcccccttgcagcaatgctcttcccagcattacgttgcgggtaaaacggaggtcgtgtacccgacctagcagcccagggatggaaaagtcccggccgtcgctggcaataatagcgggcggacgcatgtcatgagattattggaaaccaccagaatcgaatataaaaggcgaacacctttcccaattttggtttctcctgacccaaagactttaaatttaatttatttgtccctatttcaatcaattgaacaactat</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -1435,47 +1429,49 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://synbiohub.org/public/Excel2SBOL/Truncated/1</t>
+          <t>https://synbiohub.org/public/Excel2SBOL/mutations/1</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>http://examples.org/PARS/1</t>
+          <t>http://examples.org/yEGFP_Sec/1</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>PARS</t>
+          <t>yEGFP_Sec</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>origin_of_replication</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v/>
+          <t>CDS</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>No start or stop codon, for use with N-terminal secretion tag</t>
+        </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Pichia autonomously replicating sequence</t>
+          <t>Green fluorescent protein</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
+          <t>Aequorea victoria</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
           <t>Pichia pastoris</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Pichia pastoris</t>
-        </is>
-      </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>ccttcgtttgtgcggatccaattaatatttacttattttggtcaaccccaaataggttgatttcatacttggttcattcaaaaataagtagtcttttgagatctttcaatattataataaatatactataacagccgacttgtttcattttcgcgaatgttcccccagcttatcg</t>
+          <t>gtgagcaagggcgaggagctgttcaccggggtggtgcccatcctggtcgagctggacggcgacgtaaacggccacaagttcagcgtgtccggcgagggcgagggcgatgccacctacggcaagctgaccctgaagttcatctgcaccaccggcaagctgcccgtgccctggcccaccctcgtgaccaccctgacctacggcgtgcagtgcttcagccgctaccccgaccacatgaagcagcacgacttcttcaagtccgccatgcccgaaggctacgtccaggagcgcaccatcttcttcaaggacgacggcaactacaagacccgcgccgaggtgaagttcgagggcgacaccctggtgaaccgcatcgagctgaagggcatcgacttcaaggaggacggcaacatcctggggcacaagctggagtacaactacaacagccacaacgtctatatcatggccgacaagcagaagaacggcatcaaggtgaacttcaagatccgccacaacatcgaggacggcagcgtgcagctcgccgaccactaccagcagaacacccccatcggcgacggccccgtgctgctgcccgacaaccactacctgagcacccagagcgccctgagcaaagaccccaacgagaagcgcgatcacatggtcctgctggagttcgtgaccgccgccgggatcactctcggcatggacgagctgtacaag</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -1485,19 +1481,19 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://synbiohub.org/public/Excel2SBOL/mutations/1</t>
+          <t>https://synbiohub.org/public/Excel2SBOL/codon_optimisation/1</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>http://examples.org/Inulinase_u45_aMF_u916_/1</t>
+          <t>http://examples.org/aMF_u916__no_Kex/1</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Inulinase-aMFΔ</t>
+          <t>aMFΔ_no_Kex</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1505,16 +1501,20 @@
           <t>signal_peptide_region_of_CDS</t>
         </is>
       </c>
-      <c r="D32" t="n">
-        <v/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>No Kex recognition site</t>
+        </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Inulinase followed by aMFΔ</t>
-        </is>
-      </c>
-      <c r="F32" t="n">
-        <v/>
+          <t>α-mating factor no Kex recognition site</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Saccharomyces cerevisiae</t>
+        </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1523,7 +1523,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>atgaaactggcttactccctgttgctacctctggctggagtttccgctatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatctctagagaagcgt</t>
+          <t>atgagattcccatcaatttttactgctgttctgttcgccgcttctagtgcacttgccatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcacagccaaggaagaaggtgtatctctagagaagcgt</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -1531,22 +1531,26 @@
           <t>https://pubmed.ncbi.nlm.nih.gov/28252957</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr"/>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>https://synbiohub.org/public/Excel2SBOL/Truncated/1</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>http://examples.org/Killer_u45_aMF_u916_/1</t>
+          <t>http://examples.org/pAOX1/1</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Killer-aMFΔ</t>
+          <t>pAOX1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>signal_peptide_region_of_CDS</t>
+          <t>promoter</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1554,11 +1558,13 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Killer followed by aMFΔ</t>
-        </is>
-      </c>
-      <c r="F33" t="n">
-        <v/>
+          <t>Alcohol oxidase 1</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Pichia pastoris</t>
+        </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1567,7 +1573,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>atgaccaaaccaacgcaagtcttagttcgttcagtctctattttattcttcatcacactgttgcacttggttgttgcaatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatctctagagaagcgt</t>
+          <t>gatctaacatccaaagacgaaaggttgaatgaaacctttttgccatccgacatccacaggtccattctcacacataagtgccaaacgcaacaggaggggatacactagcagcagaccgttgcaaacgcaggacctccactcctcttctcctcaacacccacttttgccatcgaaaaaccagcccagttattgggcttgattggagctcgctcattccaattccttctattaggctactaacaccatgactttattagcctgtctatcctggcccccctggcgaggttcatgtttgtttatttccgaatgcaacaagctccgcattacacccgaacatcactccagatgagggctttctgagtgtggggtcaaatagtttcatgttccccaaatggcccaaaactgacagtttaaacgctgtcttggaacctaatatgacaaaagcgtgatctcatccaagatgaactaagtttggttcgttgaaatgctaacggccagttggtcaaaaagaaacttccaaaagtcggcataccgtttgtcttgtttggtattgattgacgaatgctcaaaaataatctcattaatgcttagcgcagtctctctatcgcttctgaaccccggtgcacctgtgccgaaacgcaaatggggaaacacccgctttttggatgattatgcattgtctccacattgtatgcttccaagattctggtgggaatactgctgatagcctaacgttcatgatcaaaatttaactgttctaacccctacttgacagcaatatataaacagaaggaagctgccctgtcttaaacctttttttttatcatcattattagcttactttcataattgcgactggttccaattgacaagcttttgattttaacgacttttaacgacaacttgagaagatcaaaaaacaactaattattcgaaacg</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -1575,32 +1581,34 @@
           <t>https://pubmed.ncbi.nlm.nih.gov/28252957</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr"/>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>https://synbiohub.org/public/Excel2SBOL/direct/1</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>http://examples.org/aMF_u916_/1</t>
+          <t>http://examples.org/pTPI1/1</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>aMFΔ</t>
+          <t>pTPI1</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>signal_peptide_region_of_CDS</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Pre-sequence shortened</t>
-        </is>
+          <t>promoter</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v/>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>α-mating factor, pre-sequence shortened</t>
+          <t>Triose phosphate isomerase 1</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1615,7 +1623,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>atgagatttcctagtattttcactgctgtgctatttgccgctagttcc</t>
+          <t>gtgtttaaagattacggatatttaacttacttagaataatgccatttttttgagttataataatcctacgttagtgtgagcgggatttaaactgtgaggaccttaatacattcagacacttctgcggtatcaccctacttattcccttcgagattatatctaggaacccatcaggttggtggaagattacccgttctaagacttttcagcttcctctattgatgttacacctggacaccccttttctggcatccagtttttaatcttcagtggcatgtgagattctccgaaattaactaaagcaatcacacaattctctcggataccacctcggttgaaactgacaggtggtttgttacgcatgctaatgcaaaggagcctatatacctttggctcggctgctgtaacagggaatataaagggcagcataatttaggagtttagtgaacttgcaacatttactattttcccttcttacgtaaatatttttctttttaattctaaatcaatctttttcaattttttgtttgtattcttttcttgcttaaatctataactacaaaaaacacatacataaactaaaa</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -1625,40 +1633,38 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>https://synbiohub.org/public/Excel2SBOL/Truncated/1</t>
+          <t>https://synbiohub.org/public/Excel2SBOL/mutations/1</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>http://examples.org/RFP_Sec/1</t>
+          <t>http://examples.org/attB/1</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>RFP_Sec</t>
+          <t>attB</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>CDS</t>
+          <t>site_specific_recombination_target_region</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>No start or stop codon, for use with N-terminal secretion tag</t>
+          <t>BsaI site removed</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Red fluorescent protein, BsaI removed</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Discosoma sp.</t>
-        </is>
+          <t>BxbI recognition site, BsaI site removed</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v/>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1667,7 +1673,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>gcaacttccggtatggtgtcaaagggagaggaaaataatatggctattattaaggagtttatgcgttttaaggtacatatggaaggttctgtcaacggtcacgaattcgaaattgaaggtgagggggaggggaggccatacgagggaactcagactgctaagttaaaggtcactaaaggtggtcctttacctttcgcctgggatatcctgtctccacagtttatgtacggttcaaaggcttatgtgaaacatcctgccgatatcccagattatcttaaactttctttccctgagggttttaagtgggagagggtaatgaactttgaagacggtggtgtggtcactgttactcaggactcaagtctgcaggacggtgagttcatctacaaggtgaagctgagaggtaccaattttccatcagatggtcccgtgatgcaaaaaaagacaatgggttgggaagcttctagtgaacgtatgtatcccgaagatggagctttgaaaggtgaaattaagcaaagactaaaacttaaggatggtggacattacgatgctgaagttaagacgacctacaaggccaaaaagccagtccagttgcctggagcatacaatgttaacatcaaattggatataacttcccataatgaagactataccatcgtcgagcaatacgaacgagccgaagggagacacagtactggtggtatggatgaactttataaaggatccggaaccgca</t>
+          <t>tggccgtggccgtgctcgtcctcgtcggccggcttgtcgacgacggcggtcaccgtcgtcaggatcatccgggccacaagcttgctgacagaagcctcaagaaaaaaaaaattcttcttcgactatgctggaggcagagatgatcgagccggtagttaactatatatagctaaattggttccatcac</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -1684,42 +1690,42 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>http://examples.org/pGAP/1</t>
+          <t>http://examples.org/aMF_no_EAEA/1</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>pGAP</t>
+          <t>aMF_no_EAEA</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>promoter</t>
+          <t>signal_peptide_region_of_CDS</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>BsaI site removed</t>
+          <t>No EAEA</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Glyceraldehyde-3-phosphate dehydrogenase</t>
+          <t>α-mating factor no EAEA</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
+          <t>Saccharomyces cerevisiae</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
           <t>Pichia pastoris</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Pichia pastoris</t>
-        </is>
-      </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>tttttgtagaaatgtcttggtgtcctcgtccaatcaggtagccatctctgaaatatctggctccgttgcaactccgaacgacctgctggcaacgtaaaattctccggggtaaaacttaaatgtggagtaatggaaccagaaacgtgtcttcccttctctctccttccaccgcccgttaccgtccctaggaaattttactctgctggagagcttcttctacggcccccttgcagcaatgctcttcccagcattacgttgcgggtaaaacggaggtcgtgtacccgacctagcagcccagggatggaaaagtcccggccgtcgctggcaataatagcgggcggacgcatgtcatgagattattggaaaccaccagaatcgaatataaaaggcgaacacctttcccaattttggtttctcctgacccaaagactttaaatttaatttatttgtccctatttcaatcaattgaacaactat</t>
+          <t>atgagatttccttcaatttttactgctgttttattcgcagcatcctccgcattagctgctccagtcaacactacaacagaagatgaaacggcacaaattccggctgaagctgtcatcggttactcagatttagaaggggatttcgatgttgctgttttgccattttccaacagcacaaataacgggttattgtttataaatactactattgccagcattgctgctaaagaagaaggggtatctctcgagaaaagag</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -1729,24 +1735,24 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>https://synbiohub.org/public/Excel2SBOL/mutations/1</t>
+          <t>https://synbiohub.org/public/Excel2SBOL/Truncated/1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>http://examples.org/pTPI1/1</t>
+          <t>http://examples.org/tAOX1/1</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>pTPI1</t>
+          <t>tAOX1</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>promoter</t>
+          <t>terminator</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1754,12 +1760,12 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Triose phosphate isomerase 1</t>
+          <t>Alcohol oxidase 1</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Saccharomyces cerevisiae</t>
+          <t>Pichia pastoris</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -1769,7 +1775,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>gtgtttaaagattacggatatttaacttacttagaataatgccatttttttgagttataataatcctacgttagtgtgagcgggatttaaactgtgaggaccttaatacattcagacacttctgcggtatcaccctacttattcccttcgagattatatctaggaacccatcaggttggtggaagattacccgttctaagacttttcagcttcctctattgatgttacacctggacaccccttttctggcatccagtttttaatcttcagtggcatgtgagattctccgaaattaactaaagcaatcacacaattctctcggataccacctcggttgaaactgacaggtggtttgttacgcatgctaatgcaaaggagcctatatacctttggctcggctgctgtaacagggaatataaagggcagcataatttaggagtttagtgaacttgcaacatttactattttcccttcttacgtaaatatttttctttttaattctaaatcaatctttttcaattttttgtttgtattcttttcttgcttaaatctataactacaaaaaacacatacataaactaaaa</t>
+          <t>tcaagaggatgtcagaatgccatttgcctgagagatgcaggcttcatttttgatacttttttatttgtaacctatatagtataggattttttttgtcattttgtttcttctcgtacgagcttgctcctgatcagcctatctcgcagctgatgaatatcttgtggtaggggtttgggaaaatcattcgagtttgatgtttttcttggtatttcccactcctcttcagagtacagaagattaagtgaga</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -1779,38 +1785,38 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>https://synbiohub.org/public/Excel2SBOL/mutations/1</t>
+          <t>https://synbiohub.org/public/Excel2SBOL/direct/1</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>http://examples.org/attB/1</t>
+          <t>http://examples.org/PARS/1</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>attB</t>
+          <t>PARS</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>site_specific_recombination_target_region</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>BsaI site removed</t>
-        </is>
+          <t>origin_of_replication</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v/>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>BxbI recognition site, BsaI site removed</t>
-        </is>
-      </c>
-      <c r="F38" t="n">
-        <v/>
+          <t>Pichia autonomously replicating sequence</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Pichia pastoris</t>
+        </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1819,7 +1825,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>tggccgtggccgtgctcgtcctcgtcggccggcttgtcgacgacggcggtcaccgtcgtcaggatcatccgggccacaagcttgctgacagaagcctcaagaaaaaaaaaattcttcttcgactatgctggaggcagagatgatcgagccggtagttaactatatatagctaaattggttccatcac</t>
+          <t>ccttcgtttgtgcggatccaattaatatttacttattttggtcaaccccaaataggttgatttcatacttggttcattcaaaaataagtagtcttttgagatctttcaatattataataaatatactataacagccgacttgtttcattttcgcgaatgttcccccagcttatcg</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -1836,27 +1842,25 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>http://examples.org/pENO1/1</t>
+          <t>http://examples.org/aMF/1</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>pENO1</t>
+          <t>aMF</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>promoter</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>BsaI and BsmBI site removed</t>
-        </is>
+          <t>signal_peptide_region_of_CDS</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v/>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Enolase 1</t>
+          <t>α-mating factor</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1871,7 +1875,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>agaaagcatactatactattcgacattcctttcaatcctggaattaacagtcacttttaaaaaagacatctaccgtgaaggtgccgtagagtatcgcgttaccatatcgccaaaaactgatatacgccgcggaaaccaggcaaacaattgaaaagaaaaattttgaggaactctctgcatcgaagccgtctagagttaccactagtcagatgccgcgggcacttgagcacctcatgcacagcaataacacaacacaatggttagtagcaacctgaattcggtcattgatgcatgcatgtgccgtgaagcgggacaaccagaaaagtcgtctataaatgccggcacgtgcgatcatcgtggcggggttttaagagtgcatatcacaaattgtcgcattaccgcggaaccgccagatattcattacttgacgcaaaagcgtttgaaataatgacgaaaaagaaggaagaaaaaaaaagaaaaataccgcttctaggcgggttatctactgatccgagcttccactaggatagcacccaaacacctgcatatttggacgacctttacttacaccaccaaaaaccactttcgcctctcccgcccctgataacgtccactaattgagcgattacctgagcggtcctcttttgtttgcagcatgagacttgcatactgcaaatcgtaagtagcaacctctcaaggtcaaaactgtatggaaaccttgtcacctcacttaattctagctagcctaccctgcaagtcaagagctctccgtgattcctagccacctcaaggtatgcctctccccggaaactgtggccttttctggcacacatgatctccacgatttcaacatataaatagcttttgataatggcaatattaatcaaatttattttacttctttcttgtaacatctctcttgtaatcccttattccttctagctatttttcataaaaaaccaagcaactgcttatcaacacacaaacactaaatcaaa</t>
+          <t>atgagatttccttcaatttttactgctgttttattcgcagcatcctccgcattagctgctccagtcaacactacaacagaagatgaaacggcacaaattccggctgaagctgtcatcggttactcagatttagaaggggatttcgatgttgctgttttgccattttccaacagcacaaataacgggttattgtttataaatactactattgccagcattgctgctaaagaagaaggggtatctctcgagaaaagagaggctgaagct</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -1888,33 +1892,29 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>http://examples.org/yEGFP_Sec/1</t>
+          <t>http://examples.org/aAmylase_u45_aMF_u916_/1</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>yEGFP_Sec</t>
+          <t>aAmylase-aMFΔ</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>CDS</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>No start or stop codon, for use with N-terminal secretion tag</t>
-        </is>
+          <t>signal_peptide_region_of_CDS</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v/>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Green fluorescent protein</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Aequorea victoria</t>
-        </is>
+          <t>α-Amylase followed by aMFΔ</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v/>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>gtgagcaagggcgaggagctgttcaccggggtggtgcccatcctggtcgagctggacggcgacgtaaacggccacaagttcagcgtgtccggcgagggcgagggcgatgccacctacggcaagctgaccctgaagttcatctgcaccaccggcaagctgcccgtgccctggcccaccctcgtgaccaccctgacctacggcgtgcagtgcttcagccgctaccccgaccacatgaagcagcacgacttcttcaagtccgccatgcccgaaggctacgtccaggagcgcaccatcttcttcaaggacgacggcaactacaagacccgcgccgaggtgaagttcgagggcgacaccctggtgaaccgcatcgagctgaagggcatcgacttcaaggaggacggcaacatcctggggcacaagctggagtacaactacaacagccacaacgtctatatcatggccgacaagcagaagaacggcatcaaggtgaacttcaagatccgccacaacatcgaggacggcagcgtgcagctcgccgaccactaccagcagaacacccccatcggcgacggccccgtgctgctgcccgacaaccactacctgagcacccagagcgccctgagcaaagaccccaacgagaagcgcgatcacatggtcctgctggagttcgtgaccgccgccgggatcactctcggcatggacgagctgtacaag</t>
+          <t>atggtggcatggtggtccttattcttatatggtcttcaagttgctgctcctgcccttgctatgagatttcctagtattttcactgctgtgctatttgccgctagttccgctctagctgctccagttaatactactactgaagatgaattggagggtgacttcgatgttgctgttctgcctttttccgcttctatcgcagccaaggaagaaggtgtatctctagagaagcgt</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>https://synbiohub.org/public/Excel2SBOL/codon_optimisation/1</t>
+          <t>https://synbiohub.org/public/Excel2SBOL/Composite/1</t>
         </is>
       </c>
     </row>

</xml_diff>